<commit_message>
feat: implement Excel import functionality for checklist creation and enhance deletion handling
</commit_message>
<xml_diff>
--- a/public/files/Create Checklist Template.xlsx
+++ b/public/files/Create Checklist Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427D0BD1-DD77-4FBD-9AA7-6A64B0CBC169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D6603F-6C44-4875-B52D-C4ECCD1EEFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Required</t>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -93,7 +93,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -438,7 +438,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>